<commit_message>
Borrado de ficheros .xlsx temporales
</commit_message>
<xml_diff>
--- a/Fase3_1_Nuria.xlsx
+++ b/Fase3_1_Nuria.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t xml:space="preserve">NOMBRE COLUMNA</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">DTYPE</t>
   </si>
   <si>
+    <t xml:space="preserve">VALUES</t>
+  </si>
+  <si>
     <t xml:space="preserve">TABLA</t>
   </si>
   <si>
@@ -40,30 +43,70 @@
     <t xml:space="preserve">ATTRIBUTES</t>
   </si>
   <si>
+    <t xml:space="preserve">???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT NULL, UNIQUE, AUTO_INCREMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Age</t>
   </si>
   <si>
     <t xml:space="preserve">Attrition</t>
   </si>
   <si>
+    <t xml:space="preserve">boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[True, False]</t>
+  </si>
+  <si>
     <t xml:space="preserve">BusinessTravel</t>
   </si>
   <si>
+    <t xml:space="preserve">object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[nan, 'travel_rarely', 'travel_frequently', 'non-travel']</t>
+  </si>
+  <si>
     <t xml:space="preserve">DailyRate</t>
   </si>
   <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
     <t xml:space="preserve">Department</t>
   </si>
   <si>
+    <t xml:space="preserve">[nan, ' Research &amp; Development ', ' Sales ', ' Human Resources ']</t>
+  </si>
+  <si>
     <t xml:space="preserve">DistanceFromHome</t>
   </si>
   <si>
+    <t xml:space="preserve">int64</t>
+  </si>
+  <si>
     <t xml:space="preserve">Education</t>
   </si>
   <si>
+    <t xml:space="preserve">[1, 2, 3, 4, 5]</t>
+  </si>
+  <si>
     <t xml:space="preserve">EducationField</t>
   </si>
   <si>
+    <t xml:space="preserve">[nan, 'Life Sciences', 'Technical Degree', 'Medical', 'Other',
+       'Marketing', 'Human Resources']</t>
+  </si>
+  <si>
     <t xml:space="preserve">employeecount</t>
   </si>
   <si>
@@ -73,9 +116,15 @@
     <t xml:space="preserve">EnvironmentSatisfaction</t>
   </si>
   <si>
+    <t xml:space="preserve">[1, 2, 3, 4]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
+    <t xml:space="preserve">['H','M']</t>
+  </si>
+  <si>
     <t xml:space="preserve">HourlyRate</t>
   </si>
   <si>
@@ -92,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">MaritalStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Married', 'Divorced', 'Single']</t>
   </si>
   <si>
     <t xml:space="preserve">MonthlyIncome</t>
@@ -198,12 +250,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -240,13 +304,45 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -266,241 +362,355 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G43"/>
+  <dimension ref="B1:H43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="53.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.88"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>6</v>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>7</v>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
-        <v>17</v>
+      <c r="D14" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>18</v>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>19</v>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>20</v>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>21</v>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>22</v>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>23</v>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>24</v>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>25</v>
+      <c r="B22" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>26</v>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>27</v>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>28</v>
+      <c r="B25" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>29</v>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
-        <v>30</v>
+      <c r="B27" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>31</v>
+      <c r="B28" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>32</v>
+      <c r="B29" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>33</v>
+      <c r="B30" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>34</v>
+      <c r="B31" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>35</v>
+      <c r="B32" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>36</v>
+      <c r="B33" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>37</v>
+      <c r="B34" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>38</v>
+      <c r="B35" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>39</v>
+      <c r="B36" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>40</v>
+      <c r="B37" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
-        <v>41</v>
+      <c r="B38" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
-        <v>42</v>
+      <c r="B39" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
-        <v>43</v>
+      <c r="B40" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>44</v>
+      <c r="B41" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
-        <v>45</v>
+      <c r="B42" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
-        <v>46</v>
+      <c r="B43" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>